<commit_message>
China Southern RPA done
</commit_message>
<xml_diff>
--- a/ChinaSouthernCargo/Test.xlsx
+++ b/ChinaSouthernCargo/Test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pvanausdeln\Dropbox (Blume Global)\Documents\UiPath\AirCarrierRPA\SkyTeamCargo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pvanausdeln\Dropbox (Blume Global)\Documents\UiPath\AirCarrierRPA\ChinaSouthernCargo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t>WONumber</t>
   </si>
@@ -35,61 +35,58 @@
     <t>Waybill Number</t>
   </si>
   <si>
-    <t>112-50278944</t>
-  </si>
-  <si>
-    <t>T390005721</t>
-  </si>
-  <si>
-    <t>112-52245454</t>
-  </si>
-  <si>
-    <t>T390005719</t>
-  </si>
-  <si>
-    <t>112-52127250</t>
-  </si>
-  <si>
-    <t>T980003335</t>
-  </si>
-  <si>
-    <t>112-52319326</t>
-  </si>
-  <si>
-    <t>DJBNAA4138379</t>
-  </si>
-  <si>
-    <t>112-99910392</t>
-  </si>
-  <si>
-    <t>T13605155</t>
-  </si>
-  <si>
-    <t>112-52319260</t>
-  </si>
-  <si>
-    <t>DJJFKA4136799</t>
-  </si>
-  <si>
-    <t>112-52319374</t>
-  </si>
-  <si>
-    <t>DJJFKA4136655</t>
-  </si>
-  <si>
-    <t>112-52127574</t>
-  </si>
-  <si>
-    <t>DJSINA4136390</t>
-  </si>
-  <si>
-    <t>DJSINA4135579</t>
-  </si>
-  <si>
-    <t>112-52127471</t>
-  </si>
-  <si>
-    <t>DJBKKA4135104</t>
+    <t>784-69784750</t>
+  </si>
+  <si>
+    <t>784-24772392</t>
+  </si>
+  <si>
+    <t>T040384489</t>
+  </si>
+  <si>
+    <t>784-40756752</t>
+  </si>
+  <si>
+    <t>784-22861764</t>
+  </si>
+  <si>
+    <t>DJMFEA4228904</t>
+  </si>
+  <si>
+    <t>23G0010440</t>
+  </si>
+  <si>
+    <t>784-69735175</t>
+  </si>
+  <si>
+    <t>DJORDA4228886</t>
+  </si>
+  <si>
+    <t>DJORDA4228898</t>
+  </si>
+  <si>
+    <t>784-69735061</t>
+  </si>
+  <si>
+    <t>T210010236</t>
+  </si>
+  <si>
+    <t>784-22862416</t>
+  </si>
+  <si>
+    <t>DJAMSA4227503</t>
+  </si>
+  <si>
+    <t>784-69785866</t>
+  </si>
+  <si>
+    <t>DJAMSA4225276</t>
+  </si>
+  <si>
+    <t>784-69734884</t>
+  </si>
+  <si>
+    <t>T260053631</t>
   </si>
 </sst>
 </file>
@@ -436,88 +433,88 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>4</v>
+      <c r="B2" s="1">
+        <v>2042807795</v>
+      </c>
+      <c r="C2" s="1">
+        <v>2042807795</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>2052898015</v>
+      </c>
+      <c r="C4">
+        <v>2052898015</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
         <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5">
-        <v>218966143</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
         <v>11</v>
       </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" t="s">
-        <v>12</v>
+      <c r="C6">
+        <v>2042806833</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C7">
-        <v>2061837995</v>
+        <v>2042806834</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8">
-        <v>2061837975</v>
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C9">
-        <v>2711773129</v>
+        <v>2482456744</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -525,21 +522,21 @@
         <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C10">
-        <v>2711773128</v>
+        <v>2482458634</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
         <v>20</v>
       </c>
-      <c r="B11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11">
-        <v>2840511258</v>
+      <c r="C11" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>